<commit_message>
combine algo with visualisation
</commit_message>
<xml_diff>
--- a/2019 Showcase Space and Logistics Requirements_7Aug2019.xlsx
+++ b/2019 Showcase Space and Logistics Requirements_7Aug2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shinj\Desktop\2dpacking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tharun_work\Term_5\ESC Term 5\ESC Project\ESC_ALGORITHM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80444472-20E9-4BE3-8A89-CC040E9E48DE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0696B964-CDF4-422D-99B0-A15561C4BC13}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 Request" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="329">
   <si>
     <t>Type of Prototype:</t>
   </si>
@@ -1055,6 +1055,9 @@
   </si>
   <si>
     <t>Showcase Space Needed: L x W x H</t>
+  </si>
+  <si>
+    <t>Tag</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1201,11 +1204,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1245,9 +1257,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1345,6 +1354,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1705,120 +1720,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S72"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E2"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T70" sqref="T70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="1" max="1" width="9.08984375" style="3"/>
     <col min="2" max="2" width="20" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="4.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="3.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.31640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="4.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.31640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.08984375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="3.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="12.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.44140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="15.44140625" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.109375" style="2"/>
+    <col min="14" max="14" width="5.6796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.453125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="15.453125" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="49" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="50" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="51" t="s">
         <v>327</v>
       </c>
-      <c r="F1" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="48" t="s">
+      <c r="F1" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48" t="s">
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="49" t="s">
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="50" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="37" t="s">
+      <c r="T1" s="47" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="M2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="46" t="s">
         <v>320</v>
       </c>
-      <c r="P2" s="47" t="s">
+      <c r="P2" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="49"/>
-    </row>
-    <row r="3" spans="1:19" s="21" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="50"/>
+      <c r="T2" s="48"/>
+    </row>
+    <row r="3" spans="1:20" s="20" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>314</v>
       </c>
       <c r="C3" s="7"/>
@@ -1849,25 +1868,28 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="15"/>
-    </row>
-    <row r="4" spans="1:19" s="21" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S3" s="14"/>
+      <c r="T3" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="20" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>261</v>
       </c>
       <c r="G4" s="13">
@@ -1879,7 +1901,7 @@
       <c r="I4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="13">
@@ -1903,30 +1925,33 @@
       <c r="Q4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="19" t="s">
         <v>262</v>
       </c>
       <c r="S4" s="13" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" s="21" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T4" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="20" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>105</v>
       </c>
       <c r="G5" s="13">
@@ -1938,7 +1963,7 @@
       <c r="I5" s="13">
         <v>2</v>
       </c>
-      <c r="J5" s="19"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="13">
         <v>1</v>
       </c>
@@ -1960,30 +1985,33 @@
       <c r="Q5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="24" t="s">
+      <c r="R5" s="23" t="s">
         <v>301</v>
       </c>
       <c r="S5" s="13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" s="21" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T5" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="20" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>270</v>
       </c>
       <c r="G6" s="13">
@@ -1995,7 +2023,7 @@
       <c r="I6" s="13">
         <v>1</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="13" t="s">
@@ -2019,28 +2047,31 @@
       <c r="Q6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R6" s="20"/>
+      <c r="R6" s="19"/>
       <c r="S6" s="13" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" s="21" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T6" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="34">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>199</v>
       </c>
       <c r="G7" s="13">
@@ -2050,7 +2081,7 @@
       <c r="I7" s="13">
         <v>2</v>
       </c>
-      <c r="J7" s="19"/>
+      <c r="J7" s="18"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13" t="s">
@@ -2060,28 +2091,31 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="20"/>
+      <c r="R7" s="19"/>
       <c r="S7" s="13" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" s="21" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T7" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="13">
@@ -2093,7 +2127,7 @@
       <c r="I8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="19"/>
+      <c r="J8" s="18"/>
       <c r="K8" s="13">
         <v>1</v>
       </c>
@@ -2113,28 +2147,31 @@
         <v>1</v>
       </c>
       <c r="Q8" s="13"/>
-      <c r="R8" s="20"/>
+      <c r="R8" s="19"/>
       <c r="S8" s="13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" s="21" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T8" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>277</v>
       </c>
       <c r="G9" s="13">
@@ -2146,7 +2183,7 @@
       <c r="I9" s="13">
         <v>1</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="13"/>
@@ -2162,30 +2199,33 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="24" t="s">
+      <c r="R9" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="S9" s="33" t="s">
+      <c r="S9" s="32" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" s="21" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T9" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="20" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="34">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>174</v>
       </c>
       <c r="G10" s="13">
@@ -2197,7 +2237,7 @@
       <c r="I10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K10" s="13" t="s">
@@ -2221,18 +2261,21 @@
       <c r="Q10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R10" s="20" t="s">
+      <c r="R10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="S10" s="13" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" s="21" customFormat="1" ht="170.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T10" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="20" customFormat="1" ht="170.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>307</v>
       </c>
       <c r="C11" s="7"/>
@@ -2269,27 +2312,30 @@
       <c r="R11" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="S11" s="15" t="s">
+      <c r="S11" s="14" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" s="21" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T11" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="18" t="s">
         <v>229</v>
       </c>
       <c r="G12" s="13">
@@ -2299,7 +2345,7 @@
       <c r="I12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="19"/>
+      <c r="J12" s="18"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13" t="s">
@@ -2309,28 +2355,31 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="20"/>
+      <c r="R12" s="19"/>
       <c r="S12" s="13" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" s="21" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T12" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="34">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>112</v>
       </c>
       <c r="G13" s="13">
@@ -2342,7 +2391,7 @@
       <c r="I13" s="13">
         <v>2</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="18" t="s">
         <v>113</v>
       </c>
       <c r="K13" s="13">
@@ -2364,30 +2413,33 @@
         <v>3</v>
       </c>
       <c r="Q13" s="13"/>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="19" t="s">
         <v>114</v>
       </c>
       <c r="S13" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" s="21" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T13" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="34">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="18" t="s">
         <v>129</v>
       </c>
       <c r="G14" s="13">
@@ -2399,7 +2451,7 @@
       <c r="I14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="18" t="s">
         <v>130</v>
       </c>
       <c r="K14" s="13" t="s">
@@ -2423,30 +2475,33 @@
       <c r="Q14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="20" t="s">
+      <c r="R14" s="19" t="s">
         <v>27</v>
       </c>
       <c r="S14" s="13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" s="21" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T14" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="20" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A15" s="13">
         <v>13</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="34">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="18" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="13">
@@ -2458,7 +2513,7 @@
       <c r="I15" s="13">
         <v>1</v>
       </c>
-      <c r="J15" s="19"/>
+      <c r="J15" s="18"/>
       <c r="K15" s="13" t="s">
         <v>27</v>
       </c>
@@ -2480,28 +2535,31 @@
       <c r="Q15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="20"/>
+      <c r="R15" s="19"/>
       <c r="S15" s="13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" s="21" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T15" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="20" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="18" t="s">
         <v>202</v>
       </c>
       <c r="G16" s="13">
@@ -2511,7 +2569,7 @@
       <c r="I16" s="13">
         <v>1</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="18"/>
       <c r="K16" s="13">
         <v>2</v>
       </c>
@@ -2525,28 +2583,31 @@
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="20"/>
+      <c r="R16" s="19"/>
       <c r="S16" s="13" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" s="21" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T16" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="20" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="34">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>236</v>
       </c>
       <c r="G17" s="13">
@@ -2556,7 +2617,7 @@
       <c r="I17" s="13">
         <v>1</v>
       </c>
-      <c r="J17" s="19"/>
+      <c r="J17" s="18"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13" t="s">
@@ -2578,24 +2639,27 @@
       <c r="S17" s="13" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" s="21" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T17" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="20" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A18" s="13">
         <v>16</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="18" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="13">
@@ -2607,7 +2671,7 @@
       <c r="I18" s="13">
         <v>1</v>
       </c>
-      <c r="J18" s="19"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="13" t="s">
         <v>27</v>
       </c>
@@ -2629,28 +2693,31 @@
       <c r="Q18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="20"/>
+      <c r="R18" s="19"/>
       <c r="S18" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" s="21" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T18" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="20" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A19" s="13">
         <v>17</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="18" t="s">
         <v>48</v>
       </c>
       <c r="G19" s="13">
@@ -2662,7 +2729,7 @@
       <c r="I19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="19"/>
+      <c r="J19" s="18"/>
       <c r="K19" s="13" t="s">
         <v>27</v>
       </c>
@@ -2684,26 +2751,29 @@
       <c r="Q19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R19" s="20"/>
+      <c r="R19" s="19"/>
       <c r="S19" s="13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" s="21" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T19" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A20" s="13">
         <v>18</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="18" t="s">
+      <c r="C20" s="21"/>
+      <c r="D20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="18" t="s">
         <v>51</v>
       </c>
       <c r="G20" s="13">
@@ -2715,7 +2785,7 @@
       <c r="I20" s="13">
         <v>1</v>
       </c>
-      <c r="J20" s="19"/>
+      <c r="J20" s="18"/>
       <c r="K20" s="13" t="s">
         <v>27</v>
       </c>
@@ -2737,81 +2807,87 @@
       <c r="Q20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="20" t="s">
+      <c r="R20" s="19" t="s">
         <v>52</v>
       </c>
       <c r="S20" s="13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" s="21" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25">
+      <c r="T20" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A21" s="24">
         <v>19</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="26">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="G21" s="25">
-        <v>2</v>
-      </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25">
-        <v>1</v>
-      </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="O21" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="P21" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q21" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="R21" s="24" t="s">
+      <c r="G21" s="24">
+        <v>2</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24">
+        <v>1</v>
+      </c>
+      <c r="J21" s="27"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="P21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="R21" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="S21" s="29">
+      <c r="S21" s="28">
         <v>43649</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" s="21" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T21" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A22" s="13">
         <v>20</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="19" t="s">
+      <c r="C22" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="13">
@@ -2823,7 +2899,7 @@
       <c r="I22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K22" s="13" t="s">
@@ -2847,28 +2923,31 @@
       <c r="Q22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R22" s="20" t="s">
+      <c r="R22" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="S22" s="34" t="s">
+      <c r="S22" s="33" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" s="21" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T22" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="20" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A23" s="13">
         <v>21</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="18" t="s">
+      <c r="C23" s="18"/>
+      <c r="D23" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="18" t="s">
         <v>214</v>
       </c>
       <c r="G23" s="13">
@@ -2878,7 +2957,7 @@
       <c r="I23" s="13">
         <v>1</v>
       </c>
-      <c r="J23" s="19"/>
+      <c r="J23" s="18"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13" t="s">
@@ -2888,28 +2967,31 @@
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="20"/>
+      <c r="R23" s="19"/>
       <c r="S23" s="13" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" s="30" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T23" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="29" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A24" s="13">
         <v>22</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="18" t="s">
         <v>61</v>
       </c>
       <c r="G24" s="13">
@@ -2921,7 +3003,7 @@
       <c r="I24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="18"/>
       <c r="K24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2943,28 +3025,31 @@
       <c r="Q24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R24" s="23" t="s">
+      <c r="R24" s="22" t="s">
         <v>266</v>
       </c>
       <c r="S24" s="13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" s="21" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T24" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A25" s="13">
         <v>23</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="18" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="18" t="s">
         <v>65</v>
       </c>
       <c r="G25" s="13">
@@ -2974,7 +3059,7 @@
       <c r="I25" s="13">
         <v>1</v>
       </c>
-      <c r="J25" s="19"/>
+      <c r="J25" s="18"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13" t="s">
@@ -2984,26 +3069,29 @@
       <c r="O25" s="13"/>
       <c r="P25" s="13"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="20"/>
+      <c r="R25" s="19"/>
       <c r="S25" s="13" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" s="21" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T25" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A26" s="13">
         <v>24</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="18" t="s">
+      <c r="C26" s="18"/>
+      <c r="D26" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="13">
@@ -3013,7 +3101,7 @@
       <c r="I26" s="13">
         <v>1</v>
       </c>
-      <c r="J26" s="19"/>
+      <c r="J26" s="18"/>
       <c r="K26" s="13">
         <v>1</v>
       </c>
@@ -3025,26 +3113,29 @@
       <c r="O26" s="13"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="20"/>
+      <c r="R26" s="19"/>
       <c r="S26" s="13" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" s="21" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T26" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A27" s="13">
         <v>25</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="18" t="s">
+      <c r="C27" s="21"/>
+      <c r="D27" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="18" t="s">
         <v>177</v>
       </c>
       <c r="G27" s="13">
@@ -3056,7 +3147,7 @@
       <c r="I27" s="13">
         <v>2</v>
       </c>
-      <c r="J27" s="19"/>
+      <c r="J27" s="18"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
@@ -3064,26 +3155,29 @@
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="20"/>
+      <c r="R27" s="19"/>
       <c r="S27" s="13" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" s="21" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T27" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A28" s="13">
         <v>26</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="19" t="s">
+      <c r="C28" s="34"/>
+      <c r="D28" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="18" t="s">
         <v>172</v>
       </c>
       <c r="G28" s="13">
@@ -3093,7 +3187,7 @@
       <c r="I28" s="13">
         <v>1</v>
       </c>
-      <c r="J28" s="19"/>
+      <c r="J28" s="18"/>
       <c r="K28" s="13">
         <v>1</v>
       </c>
@@ -3109,30 +3203,33 @@
       <c r="Q28" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="R28" s="20" t="s">
+      <c r="R28" s="19" t="s">
         <v>317</v>
       </c>
       <c r="S28" s="13" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" s="21" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T28" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A29" s="13">
         <v>27</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="18" t="s">
         <v>141</v>
       </c>
       <c r="G29" s="13">
@@ -3144,7 +3241,7 @@
       <c r="I29" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K29" s="13" t="s">
@@ -3168,26 +3265,29 @@
       <c r="Q29" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R29" s="20"/>
+      <c r="R29" s="19"/>
       <c r="S29" s="13" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" s="21" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T29" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" s="20" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A30" s="13">
         <v>28</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18" t="s">
+      <c r="C30" s="18"/>
+      <c r="D30" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="13">
@@ -3199,7 +3299,7 @@
       <c r="I30" s="13">
         <v>1</v>
       </c>
-      <c r="J30" s="19"/>
+      <c r="J30" s="18"/>
       <c r="K30" s="13" t="s">
         <v>27</v>
       </c>
@@ -3221,30 +3321,33 @@
       <c r="Q30" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R30" s="24" t="s">
+      <c r="R30" s="23" t="s">
         <v>81</v>
       </c>
       <c r="S30" s="13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T30" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A31" s="13">
         <v>29</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="18" t="s">
         <v>29</v>
       </c>
       <c r="G31" s="13">
@@ -3256,7 +3359,7 @@
       <c r="I31" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J31" s="19"/>
+      <c r="J31" s="18"/>
       <c r="K31" s="13" t="s">
         <v>27</v>
       </c>
@@ -3278,28 +3381,31 @@
       <c r="Q31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="R31" s="20"/>
+      <c r="R31" s="19"/>
       <c r="S31" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T31" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A32" s="13">
         <v>30</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="19" t="s">
+      <c r="F32" s="18" t="s">
         <v>221</v>
       </c>
       <c r="G32" s="13">
@@ -3309,7 +3415,7 @@
       <c r="I32" s="13">
         <v>1</v>
       </c>
-      <c r="J32" s="19"/>
+      <c r="J32" s="18"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13">
@@ -3319,28 +3425,31 @@
       <c r="O32" s="13"/>
       <c r="P32" s="13"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="20"/>
+      <c r="R32" s="19"/>
       <c r="S32" s="13" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T32" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A33" s="13">
         <v>31</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="18" t="s">
         <v>254</v>
       </c>
       <c r="G33" s="13">
@@ -3352,7 +3461,7 @@
       <c r="I33" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K33" s="13" t="s">
@@ -3376,28 +3485,31 @@
       <c r="Q33" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R33" s="20"/>
+      <c r="R33" s="19"/>
       <c r="S33" s="13" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A34" s="13">
         <v>32</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="18" t="s">
         <v>146</v>
       </c>
       <c r="G34" s="13">
@@ -3409,7 +3521,7 @@
       <c r="I34" s="13">
         <v>4</v>
       </c>
-      <c r="J34" s="19" t="s">
+      <c r="J34" s="18" t="s">
         <v>153</v>
       </c>
       <c r="K34" s="13">
@@ -3433,30 +3545,33 @@
       <c r="Q34" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R34" s="20" t="s">
+      <c r="R34" s="19" t="s">
         <v>147</v>
       </c>
       <c r="S34" s="13" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T34" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A35" s="13">
         <v>33</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="18" t="s">
         <v>169</v>
       </c>
       <c r="G35" s="13">
@@ -3464,7 +3579,7 @@
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
-      <c r="J35" s="19"/>
+      <c r="J35" s="18"/>
       <c r="K35" s="13">
         <v>1</v>
       </c>
@@ -3482,30 +3597,33 @@
       <c r="Q35" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R35" s="20" t="s">
+      <c r="R35" s="19" t="s">
         <v>296</v>
       </c>
       <c r="S35" s="13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T35" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A36" s="13">
         <v>34</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="18" t="s">
         <v>108</v>
       </c>
       <c r="G36" s="13">
@@ -3517,7 +3635,7 @@
       <c r="I36" s="13">
         <v>1</v>
       </c>
-      <c r="J36" s="19"/>
+      <c r="J36" s="18"/>
       <c r="K36" s="13" t="s">
         <v>27</v>
       </c>
@@ -3539,30 +3657,33 @@
       <c r="Q36" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R36" s="20" t="s">
+      <c r="R36" s="19" t="s">
         <v>27</v>
       </c>
       <c r="S36" s="13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T36" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A37" s="13">
         <v>35</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="18" t="s">
         <v>57</v>
       </c>
       <c r="G37" s="13">
@@ -3572,7 +3693,7 @@
         <v>27</v>
       </c>
       <c r="I37" s="13"/>
-      <c r="J37" s="19"/>
+      <c r="J37" s="18"/>
       <c r="K37" s="13" t="s">
         <v>27</v>
       </c>
@@ -3594,30 +3715,33 @@
       <c r="Q37" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="R37" s="20" t="s">
+      <c r="R37" s="19" t="s">
         <v>101</v>
       </c>
       <c r="S37" s="13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T37" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A38" s="13">
         <v>36</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="18" t="s">
         <v>233</v>
       </c>
       <c r="G38" s="13">
@@ -3627,7 +3751,7 @@
       <c r="I38" s="13">
         <v>2</v>
       </c>
-      <c r="J38" s="19"/>
+      <c r="J38" s="18"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13">
         <v>1</v>
@@ -3641,30 +3765,33 @@
       <c r="O38" s="13"/>
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="20" t="s">
+      <c r="R38" s="19" t="s">
         <v>319</v>
       </c>
       <c r="S38" s="13" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T38" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A39" s="13">
         <v>37</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="18" t="s">
         <v>224</v>
       </c>
       <c r="G39" s="13">
@@ -3674,7 +3801,7 @@
       <c r="I39" s="13">
         <v>1</v>
       </c>
-      <c r="J39" s="19"/>
+      <c r="J39" s="18"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
       <c r="M39" s="13">
@@ -3684,28 +3811,31 @@
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="20"/>
+      <c r="R39" s="19"/>
       <c r="S39" s="13" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T39" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A40" s="13">
         <v>38</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="31" t="s">
+      <c r="D40" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="18" t="s">
         <v>24</v>
       </c>
       <c r="G40" s="13">
@@ -3715,7 +3845,7 @@
       <c r="I40" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J40" s="19"/>
+      <c r="J40" s="18"/>
       <c r="K40" s="13" t="s">
         <v>27</v>
       </c>
@@ -3737,28 +3867,31 @@
       <c r="Q40" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R40" s="32" t="s">
+      <c r="R40" s="31" t="s">
         <v>299</v>
       </c>
       <c r="S40" s="13" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T40" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A41" s="13">
         <v>39</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="18" t="s">
+      <c r="C41" s="18"/>
+      <c r="D41" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="18" t="s">
         <v>44</v>
       </c>
       <c r="G41" s="13">
@@ -3770,7 +3903,7 @@
       <c r="I41" s="13">
         <v>3</v>
       </c>
-      <c r="J41" s="19"/>
+      <c r="J41" s="18"/>
       <c r="K41" s="13">
         <v>1</v>
       </c>
@@ -3792,26 +3925,29 @@
       <c r="Q41" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R41" s="20"/>
+      <c r="R41" s="19"/>
       <c r="S41" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T41" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A42" s="13">
         <v>40</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="18" t="s">
+      <c r="C42" s="18"/>
+      <c r="D42" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="19"/>
+      <c r="F42" s="18"/>
       <c r="G42" s="13">
         <v>2</v>
       </c>
@@ -3821,7 +3957,7 @@
       <c r="I42" s="13">
         <v>2</v>
       </c>
-      <c r="J42" s="19"/>
+      <c r="J42" s="18"/>
       <c r="K42" s="13">
         <v>1</v>
       </c>
@@ -3843,26 +3979,29 @@
       <c r="Q42" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R42" s="20"/>
+      <c r="R42" s="19"/>
       <c r="S42" s="13" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T42" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A43" s="13">
         <v>41</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="18" t="s">
+      <c r="C43" s="18"/>
+      <c r="D43" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="19" t="s">
+      <c r="F43" s="18" t="s">
         <v>75</v>
       </c>
       <c r="G43" s="13">
@@ -3874,7 +4013,7 @@
       <c r="I43" s="13">
         <v>1</v>
       </c>
-      <c r="J43" s="19"/>
+      <c r="J43" s="18"/>
       <c r="K43" s="13" t="s">
         <v>27</v>
       </c>
@@ -3902,24 +4041,27 @@
       <c r="S43" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T43" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A44" s="13">
         <v>42</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="C44" s="35">
+      <c r="C44" s="34">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="18" t="s">
         <v>302</v>
       </c>
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="F44" s="19" t="s">
+      <c r="F44" s="18" t="s">
         <v>83</v>
       </c>
       <c r="G44" s="13">
@@ -3931,7 +4073,7 @@
       <c r="I44" s="13">
         <v>1</v>
       </c>
-      <c r="J44" s="19"/>
+      <c r="J44" s="18"/>
       <c r="K44" s="13" t="s">
         <v>27</v>
       </c>
@@ -3953,28 +4095,31 @@
       <c r="Q44" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R44" s="20" t="s">
+      <c r="R44" s="19" t="s">
         <v>84</v>
       </c>
       <c r="S44" s="13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T44" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A45" s="13">
         <v>43</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="18" t="s">
+      <c r="C45" s="18"/>
+      <c r="D45" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="F45" s="18" t="s">
         <v>117</v>
       </c>
       <c r="G45" s="13">
@@ -3986,7 +4131,7 @@
       <c r="I45" s="13">
         <v>1</v>
       </c>
-      <c r="J45" s="19" t="s">
+      <c r="J45" s="18" t="s">
         <v>143</v>
       </c>
       <c r="K45" s="13">
@@ -4010,28 +4155,31 @@
       <c r="Q45" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R45" s="20" t="s">
+      <c r="R45" s="19" t="s">
         <v>118</v>
       </c>
       <c r="S45" s="13" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T45" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A46" s="13">
         <v>44</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="18" t="s">
+      <c r="C46" s="18"/>
+      <c r="D46" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="F46" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G46" s="13">
@@ -4043,7 +4191,7 @@
       <c r="I46" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J46" s="19"/>
+      <c r="J46" s="18"/>
       <c r="K46" s="13">
         <v>1</v>
       </c>
@@ -4065,28 +4213,31 @@
       <c r="Q46" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R46" s="20" t="s">
+      <c r="R46" s="19" t="s">
         <v>80</v>
       </c>
       <c r="S46" s="13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" s="21" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T46" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" s="20" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A47" s="13">
         <v>45</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="19" t="s">
+      <c r="C47" s="21"/>
+      <c r="D47" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="18" t="s">
         <v>249</v>
       </c>
       <c r="G47" s="13">
@@ -4098,7 +4249,7 @@
       <c r="I47" s="13">
         <v>3</v>
       </c>
-      <c r="J47" s="19"/>
+      <c r="J47" s="18"/>
       <c r="K47" s="13">
         <v>2</v>
       </c>
@@ -4120,28 +4271,31 @@
       <c r="Q47" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R47" s="20" t="s">
+      <c r="R47" s="19" t="s">
         <v>288</v>
       </c>
       <c r="S47" s="13" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T47" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A48" s="13">
         <v>46</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="18" t="s">
+      <c r="C48" s="18"/>
+      <c r="D48" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G48" s="13">
@@ -4153,7 +4307,7 @@
       <c r="I48" s="13">
         <v>1</v>
       </c>
-      <c r="J48" s="19"/>
+      <c r="J48" s="18"/>
       <c r="K48" s="13">
         <v>2</v>
       </c>
@@ -4175,26 +4329,29 @@
       <c r="Q48" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R48" s="20"/>
+      <c r="R48" s="19"/>
       <c r="S48" s="13" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T48" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A49" s="13">
         <v>47</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19" t="s">
+      <c r="D49" s="18"/>
+      <c r="E49" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F49" s="19"/>
+      <c r="F49" s="18"/>
       <c r="G49" s="13">
         <v>2</v>
       </c>
@@ -4204,7 +4361,7 @@
       <c r="I49" s="13">
         <v>2</v>
       </c>
-      <c r="J49" s="19" t="s">
+      <c r="J49" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K49" s="13">
@@ -4228,26 +4385,29 @@
       <c r="Q49" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R49" s="20"/>
+      <c r="R49" s="19"/>
       <c r="S49" s="13" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T49" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A50" s="13">
         <v>48</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="18" t="s">
+      <c r="C50" s="21"/>
+      <c r="D50" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="19" t="s">
+      <c r="F50" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G50" s="13">
@@ -4259,7 +4419,7 @@
       <c r="I50" s="13">
         <v>1</v>
       </c>
-      <c r="J50" s="19"/>
+      <c r="J50" s="18"/>
       <c r="K50" s="13">
         <v>1</v>
       </c>
@@ -4281,28 +4441,31 @@
       <c r="Q50" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R50" s="20"/>
+      <c r="R50" s="19"/>
       <c r="S50" s="13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" s="21" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T50" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" s="20" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A51" s="13">
         <v>49</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E51" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="F51" s="18" t="s">
         <v>34</v>
       </c>
       <c r="G51" s="13">
@@ -4314,7 +4477,7 @@
       <c r="I51" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J51" s="19"/>
+      <c r="J51" s="18"/>
       <c r="K51" s="13">
         <v>2</v>
       </c>
@@ -4334,26 +4497,29 @@
       <c r="Q51" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R51" s="20"/>
+      <c r="R51" s="19"/>
       <c r="S51" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T51" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A52" s="13">
         <v>50</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="18" t="s">
+      <c r="C52" s="18"/>
+      <c r="D52" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F52" s="18" t="s">
         <v>195</v>
       </c>
       <c r="G52" s="13">
@@ -4363,7 +4529,7 @@
       <c r="I52" s="13">
         <v>1</v>
       </c>
-      <c r="J52" s="19"/>
+      <c r="J52" s="18"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13" t="s">
@@ -4373,28 +4539,31 @@
       <c r="O52" s="13"/>
       <c r="P52" s="13"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="20"/>
+      <c r="R52" s="19"/>
       <c r="S52" s="13" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T52" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A53" s="13">
         <v>51</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="E53" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="F53" s="18" t="s">
         <v>257</v>
       </c>
       <c r="G53" s="13">
@@ -4404,7 +4573,7 @@
       <c r="I53" s="13">
         <v>1</v>
       </c>
-      <c r="J53" s="19"/>
+      <c r="J53" s="18"/>
       <c r="K53" s="13"/>
       <c r="L53" s="13"/>
       <c r="M53" s="13">
@@ -4414,26 +4583,29 @@
       <c r="O53" s="13"/>
       <c r="P53" s="13"/>
       <c r="Q53" s="13"/>
-      <c r="R53" s="20"/>
+      <c r="R53" s="19"/>
       <c r="S53" s="13" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T53" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A54" s="13">
         <v>52</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19" t="s">
+      <c r="C54" s="18"/>
+      <c r="D54" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G54" s="13">
@@ -4445,7 +4617,7 @@
       <c r="I54" s="13">
         <v>1</v>
       </c>
-      <c r="J54" s="19" t="s">
+      <c r="J54" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K54" s="13" t="s">
@@ -4469,28 +4641,31 @@
       <c r="Q54" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R54" s="20"/>
+      <c r="R54" s="19"/>
       <c r="S54" s="13" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" s="21" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T54" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A55" s="13">
         <v>53</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D55" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="19" t="s">
+      <c r="F55" s="18" t="s">
         <v>78</v>
       </c>
       <c r="G55" s="13">
@@ -4502,7 +4677,7 @@
       <c r="I55" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J55" s="19"/>
+      <c r="J55" s="18"/>
       <c r="K55" s="13" t="s">
         <v>27</v>
       </c>
@@ -4524,28 +4699,31 @@
       <c r="Q55" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R55" s="20" t="s">
+      <c r="R55" s="19" t="s">
         <v>27</v>
       </c>
       <c r="S55" s="13" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" s="21" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T55" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" s="20" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A56" s="13">
         <v>54</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19" t="s">
+      <c r="C56" s="18"/>
+      <c r="D56" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="F56" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G56" s="13">
@@ -4557,7 +4735,7 @@
       <c r="I56" s="13">
         <v>1</v>
       </c>
-      <c r="J56" s="19" t="s">
+      <c r="J56" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K56" s="13" t="s">
@@ -4581,28 +4759,31 @@
       <c r="Q56" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="R56" s="20" t="s">
+      <c r="R56" s="19" t="s">
         <v>290</v>
       </c>
       <c r="S56" s="13" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T56" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A57" s="13">
         <v>55</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="18" t="s">
+      <c r="C57" s="21"/>
+      <c r="D57" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F57" s="18" t="s">
         <v>205</v>
       </c>
       <c r="G57" s="13">
@@ -4612,7 +4793,7 @@
       <c r="I57" s="13">
         <v>1</v>
       </c>
-      <c r="J57" s="19"/>
+      <c r="J57" s="18"/>
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
       <c r="M57" s="13" t="s">
@@ -4622,28 +4803,31 @@
       <c r="O57" s="13"/>
       <c r="P57" s="13"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="20"/>
+      <c r="R57" s="19"/>
       <c r="S57" s="13" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T57" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A58" s="13">
         <v>56</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C58" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D58" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="F58" s="36" t="s">
+      <c r="F58" s="35" t="s">
         <v>208</v>
       </c>
       <c r="G58" s="13">
@@ -4653,7 +4837,7 @@
       <c r="I58" s="13">
         <v>1</v>
       </c>
-      <c r="J58" s="19"/>
+      <c r="J58" s="18"/>
       <c r="K58" s="13">
         <v>1</v>
       </c>
@@ -4665,28 +4849,31 @@
       <c r="O58" s="13"/>
       <c r="P58" s="13"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="20" t="s">
+      <c r="R58" s="19" t="s">
         <v>218</v>
       </c>
       <c r="S58" s="13" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T58" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A59" s="13">
         <v>57</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="18" t="s">
+      <c r="C59" s="21"/>
+      <c r="D59" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="F59" s="19" t="s">
+      <c r="F59" s="18" t="s">
         <v>121</v>
       </c>
       <c r="G59" s="13">
@@ -4698,7 +4885,7 @@
       <c r="I59" s="13">
         <v>1</v>
       </c>
-      <c r="J59" s="19" t="s">
+      <c r="J59" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K59" s="13">
@@ -4722,30 +4909,33 @@
       <c r="Q59" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R59" s="20" t="s">
+      <c r="R59" s="19" t="s">
         <v>154</v>
       </c>
       <c r="S59" s="13" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T59" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A60" s="13">
         <v>58</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="C60" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" s="19" t="s">
+      <c r="C60" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="E60" s="19" t="s">
+      <c r="E60" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F60" s="19" t="s">
+      <c r="F60" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G60" s="13">
@@ -4755,7 +4945,7 @@
       <c r="I60" s="13">
         <v>2</v>
       </c>
-      <c r="J60" s="19"/>
+      <c r="J60" s="18"/>
       <c r="K60" s="13">
         <v>1</v>
       </c>
@@ -4777,28 +4967,31 @@
       <c r="Q60" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R60" s="20" t="s">
+      <c r="R60" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="S60" s="34" t="s">
+      <c r="S60" s="33" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T60" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A61" s="13">
         <v>59</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19" t="s">
+      <c r="C61" s="18"/>
+      <c r="D61" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F61" s="19" t="s">
+      <c r="F61" s="18" t="s">
         <v>305</v>
       </c>
       <c r="G61" s="13">
@@ -4808,7 +5001,7 @@
         <v>1</v>
       </c>
       <c r="I61" s="13"/>
-      <c r="J61" s="19"/>
+      <c r="J61" s="18"/>
       <c r="K61" s="13">
         <v>1</v>
       </c>
@@ -4818,16 +5011,19 @@
       <c r="O61" s="13"/>
       <c r="P61" s="13"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="20"/>
-      <c r="S61" s="34" t="s">
+      <c r="R61" s="19"/>
+      <c r="S61" s="33" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" s="21" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T61" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" s="20" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A62" s="6">
         <v>60</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="15" t="s">
         <v>312</v>
       </c>
       <c r="C62" s="7"/>
@@ -4858,25 +5054,28 @@
       <c r="P62" s="6"/>
       <c r="Q62" s="6"/>
       <c r="R62" s="5"/>
-      <c r="S62" s="15"/>
-    </row>
-    <row r="63" spans="1:19" s="21" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S62" s="14"/>
+      <c r="T62" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" s="20" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A63" s="13">
         <v>61</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C63" s="18">
+      <c r="C63" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D63" s="19" t="s">
+      <c r="D63" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="F63" s="19" t="s">
+      <c r="F63" s="18" t="s">
         <v>156</v>
       </c>
       <c r="G63" s="13">
@@ -4886,7 +5085,7 @@
         <v>2</v>
       </c>
       <c r="I63" s="13"/>
-      <c r="J63" s="19" t="s">
+      <c r="J63" s="18" t="s">
         <v>161</v>
       </c>
       <c r="K63" s="13" t="s">
@@ -4910,30 +5109,33 @@
       <c r="Q63" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R63" s="20" t="s">
+      <c r="R63" s="19" t="s">
         <v>157</v>
       </c>
       <c r="S63" s="13" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T63" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A64" s="13">
         <v>62</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C64" s="18">
+      <c r="C64" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="F64" s="19" t="s">
+      <c r="F64" s="18" t="s">
         <v>136</v>
       </c>
       <c r="G64" s="13">
@@ -4945,7 +5147,7 @@
       <c r="I64" s="13">
         <v>1</v>
       </c>
-      <c r="J64" s="19" t="s">
+      <c r="J64" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K64" s="13" t="s">
@@ -4969,30 +5171,33 @@
       <c r="Q64" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R64" s="32" t="s">
+      <c r="R64" s="31" t="s">
         <v>298</v>
       </c>
       <c r="S64" s="13" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T64" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A65" s="13">
         <v>63</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="C65" s="18">
+      <c r="C65" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D65" s="19" t="s">
+      <c r="D65" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="E65" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="F65" s="19" t="s">
+      <c r="F65" s="18" t="s">
         <v>188</v>
       </c>
       <c r="G65" s="13">
@@ -5004,7 +5209,7 @@
       <c r="I65" s="13">
         <v>1</v>
       </c>
-      <c r="J65" s="19"/>
+      <c r="J65" s="18"/>
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
       <c r="M65" s="13">
@@ -5014,28 +5219,31 @@
       <c r="O65" s="13"/>
       <c r="P65" s="13"/>
       <c r="Q65" s="13"/>
-      <c r="R65" s="20"/>
+      <c r="R65" s="19"/>
       <c r="S65" s="13" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T65" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A66" s="13">
         <v>64</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C66" s="18">
+      <c r="C66" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="D66" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E66" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F66" s="19" t="s">
+      <c r="F66" s="18" t="s">
         <v>97</v>
       </c>
       <c r="G66" s="13">
@@ -5047,7 +5255,7 @@
       <c r="I66" s="13">
         <v>4</v>
       </c>
-      <c r="J66" s="19"/>
+      <c r="J66" s="18"/>
       <c r="K66" s="13">
         <v>1</v>
       </c>
@@ -5069,28 +5277,31 @@
       <c r="Q66" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R66" s="20" t="s">
+      <c r="R66" s="19" t="s">
         <v>100</v>
       </c>
       <c r="S66" s="13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T66" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A67" s="13">
         <v>65</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19" t="s">
+      <c r="C67" s="18"/>
+      <c r="D67" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E67" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F67" s="19"/>
+      <c r="F67" s="18"/>
       <c r="G67" s="13">
         <v>2</v>
       </c>
@@ -5100,7 +5311,7 @@
       <c r="I67" s="13">
         <v>2</v>
       </c>
-      <c r="J67" s="19" t="s">
+      <c r="J67" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K67" s="13" t="s">
@@ -5124,30 +5335,33 @@
       <c r="Q67" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R67" s="19" t="s">
+      <c r="R67" s="18" t="s">
         <v>245</v>
       </c>
       <c r="S67" s="13" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T67" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A68" s="13">
         <v>66</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="C68" s="18">
+      <c r="C68" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D68" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E68" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="F68" s="19" t="s">
+      <c r="F68" s="18" t="s">
         <v>150</v>
       </c>
       <c r="G68" s="13">
@@ -5157,7 +5371,7 @@
       <c r="I68" s="13">
         <v>1</v>
       </c>
-      <c r="J68" s="19"/>
+      <c r="J68" s="18"/>
       <c r="K68" s="13">
         <v>1</v>
       </c>
@@ -5175,30 +5389,33 @@
       <c r="Q68" s="13" t="s">
         <v>326</v>
       </c>
-      <c r="R68" s="20" t="s">
+      <c r="R68" s="19" t="s">
         <v>163</v>
       </c>
       <c r="S68" s="13" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T68" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A69" s="13">
         <v>67</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="C69" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D69" s="19" t="s">
+      <c r="C69" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F69" s="19" t="s">
+      <c r="F69" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G69" s="13">
@@ -5210,7 +5427,7 @@
       <c r="I69" s="13">
         <v>2</v>
       </c>
-      <c r="J69" s="19"/>
+      <c r="J69" s="18"/>
       <c r="K69" s="13">
         <v>1</v>
       </c>
@@ -5232,30 +5449,33 @@
       <c r="Q69" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R69" s="20" t="s">
+      <c r="R69" s="19" t="s">
         <v>286</v>
       </c>
       <c r="S69" s="13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T69" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A70" s="13">
         <v>68</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="18">
+      <c r="C70" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
-      <c r="D70" s="19" t="s">
+      <c r="D70" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F70" s="19" t="s">
+      <c r="F70" s="18" t="s">
         <v>92</v>
       </c>
       <c r="G70" s="13">
@@ -5267,7 +5487,7 @@
       <c r="I70" s="13">
         <v>1</v>
       </c>
-      <c r="J70" s="19"/>
+      <c r="J70" s="18"/>
       <c r="K70" s="13" t="s">
         <v>27</v>
       </c>
@@ -5289,95 +5509,78 @@
       <c r="Q70" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R70" s="20" t="s">
+      <c r="R70" s="19" t="s">
         <v>93</v>
       </c>
       <c r="S70" s="13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T70" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A71" s="6"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="7"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
-      <c r="P71" s="6"/>
-      <c r="Q71" s="6"/>
-      <c r="R71" s="5"/>
-      <c r="S71" s="15"/>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A72" s="6"/>
-      <c r="B72" s="11" t="s">
+      <c r="B71" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="9">
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="9">
         <f>SUM(G3:G70)</f>
         <v>168</v>
       </c>
-      <c r="H72" s="9">
-        <f t="shared" ref="H72:Q72" si="0">SUM(H3:H70)</f>
+      <c r="H71" s="9">
+        <f t="shared" ref="H71:Q71" si="0">SUM(H3:H70)</f>
         <v>12</v>
       </c>
-      <c r="I72" s="9">
+      <c r="I71" s="9">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="J72" s="9">
+      <c r="J71" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K72" s="9">
+      <c r="K71" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="L72" s="9">
+      <c r="L71" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="M72" s="9">
+      <c r="M71" s="9">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="N72" s="9">
+      <c r="N71" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="O72" s="9">
-        <f t="shared" ref="O72:P72" si="1">SUM(O3:O70)</f>
+      <c r="O71" s="9">
+        <f t="shared" ref="O71:P71" si="1">SUM(O3:O70)</f>
         <v>12</v>
       </c>
-      <c r="P72" s="9">
+      <c r="P71" s="9">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="Q72" s="9">
+      <c r="Q71" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R72" s="8"/>
-      <c r="S72" s="9"/>
+      <c r="R71" s="8"/>
+      <c r="S71" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q70">
     <sortCondition ref="A3:A70"/>
   </sortState>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="T1:T2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:R1"/>
@@ -5403,566 +5606,566 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="42" customWidth="1"/>
-    <col min="2" max="2" width="66.109375" style="46" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="38"/>
+    <col min="1" max="1" width="10.08984375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="66.08984375" style="45" customWidth="1"/>
+    <col min="3" max="16384" width="9.08984375" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A1" s="54" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="55" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
-        <v>1</v>
-      </c>
-      <c r="B3" s="43" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A3" s="38">
+        <v>1</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="40">
-        <v>2</v>
-      </c>
-      <c r="B4" s="44" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A4" s="39">
+        <v>2</v>
+      </c>
+      <c r="B4" s="43" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="40">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A5" s="39">
         <v>3</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="40">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="40">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A7" s="39">
         <v>5</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="40">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A8" s="39">
         <v>6</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="43" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="40">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A9" s="39">
         <v>7</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="43" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="40">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A10" s="39">
         <v>8</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="43" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A11" s="38">
         <v>9</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="42" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="40">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="40">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A13" s="39">
         <v>11</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="40">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A14" s="39">
         <v>12</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="40">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A15" s="39">
         <v>13</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="40">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A16" s="39">
         <v>14</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="40">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A17" s="39">
         <v>15</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="40">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A18" s="39">
         <v>16</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="43" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="40">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A19" s="39">
         <v>17</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="43" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="40">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A20" s="39">
         <v>18</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="41">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A21" s="40">
         <v>19</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="40">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A22" s="39">
         <v>20</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="43" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="40">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A23" s="39">
         <v>21</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="43" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="40">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A24" s="39">
         <v>22</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="43" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="40">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A25" s="39">
         <v>23</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="43" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="40">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A26" s="39">
         <v>24</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="43" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="40">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A27" s="39">
         <v>25</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="43" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="40">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="43" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="40">
-        <v>27</v>
-      </c>
-      <c r="B29" s="44" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A29" s="39">
+        <v>27</v>
+      </c>
+      <c r="B29" s="43" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="40">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A30" s="39">
         <v>28</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="43" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="40">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A31" s="39">
         <v>29</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="40">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A32" s="39">
         <v>30</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="43" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="40">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A33" s="39">
         <v>31</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="43" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="40">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A34" s="39">
         <v>32</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="43" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="40">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A35" s="39">
         <v>33</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="43" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="40">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A36" s="39">
         <v>34</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="43" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="40">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A37" s="39">
         <v>35</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="43" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="40">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A38" s="39">
         <v>36</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="43" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="40">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A39" s="39">
         <v>37</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="43" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="40">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A40" s="39">
         <v>38</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="43" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="40">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A41" s="39">
         <v>39</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="40">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A42" s="39">
         <v>40</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="40">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A43" s="39">
         <v>41</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="40">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A44" s="39">
         <v>42</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="43" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="40">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A45" s="39">
         <v>43</v>
       </c>
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="43" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="40">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A46" s="39">
         <v>44</v>
       </c>
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="43" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="40">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A47" s="39">
         <v>45</v>
       </c>
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="43" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="40">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A48" s="39">
         <v>46</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="43" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="40">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A49" s="39">
         <v>47</v>
       </c>
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="43" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="40">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A50" s="39">
         <v>48</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="43" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="40">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A51" s="39">
         <v>49</v>
       </c>
-      <c r="B51" s="44" t="s">
+      <c r="B51" s="43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="40">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A52" s="39">
         <v>50</v>
       </c>
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="43" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="40">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A53" s="39">
         <v>51</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="43" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="40">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A54" s="39">
         <v>52</v>
       </c>
-      <c r="B54" s="44" t="s">
+      <c r="B54" s="43" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="40">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A55" s="39">
         <v>53</v>
       </c>
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="43" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="40">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A56" s="39">
         <v>54</v>
       </c>
-      <c r="B56" s="44" t="s">
+      <c r="B56" s="43" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="40">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A57" s="39">
         <v>55</v>
       </c>
-      <c r="B57" s="44" t="s">
+      <c r="B57" s="43" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="40">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A58" s="39">
         <v>56</v>
       </c>
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="43" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="40">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A59" s="39">
         <v>57</v>
       </c>
-      <c r="B59" s="44" t="s">
+      <c r="B59" s="43" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="40">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A60" s="39">
         <v>58</v>
       </c>
-      <c r="B60" s="44" t="s">
+      <c r="B60" s="43" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="40">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A61" s="39">
         <v>59</v>
       </c>
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="43" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="39">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A62" s="38">
         <v>60</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="42" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="40">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A63" s="39">
         <v>61</v>
       </c>
-      <c r="B63" s="44" t="s">
+      <c r="B63" s="43" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="40">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A64" s="39">
         <v>62</v>
       </c>
-      <c r="B64" s="44" t="s">
+      <c r="B64" s="43" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="40">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A65" s="39">
         <v>63</v>
       </c>
-      <c r="B65" s="44" t="s">
+      <c r="B65" s="43" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="40">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A66" s="39">
         <v>64</v>
       </c>
-      <c r="B66" s="44" t="s">
+      <c r="B66" s="43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="40">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A67" s="39">
         <v>65</v>
       </c>
-      <c r="B67" s="44" t="s">
+      <c r="B67" s="43" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="40">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A68" s="39">
         <v>66</v>
       </c>
-      <c r="B68" s="44" t="s">
+      <c r="B68" s="43" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="40">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A69" s="39">
         <v>67</v>
       </c>
-      <c r="B69" s="44" t="s">
+      <c r="B69" s="43" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="40">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A70" s="39">
         <v>68</v>
       </c>
-      <c r="B70" s="44" t="s">
+      <c r="B70" s="43" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Major Algo bugs fixed
</commit_message>
<xml_diff>
--- a/2019 Showcase Space and Logistics Requirements_7Aug2019.xlsx
+++ b/2019 Showcase Space and Logistics Requirements_7Aug2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tharun_work\Term_5\ESC Term 5\ESC Project\ESC_ALGORITHM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thawalk\Documents\GitHub\2dpacking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0696B964-CDF4-422D-99B0-A15561C4BC13}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43643194-906F-4D81-BC7F-C1BB65FEB693}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 Request" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="328">
   <si>
     <t>Type of Prototype:</t>
   </si>
@@ -414,9 +414,6 @@
   </si>
   <si>
     <t>Proj S05 - Flotech_Tagging</t>
-  </si>
-  <si>
-    <t>Library iWall and space around it (Already confirmed with SUTD Library)</t>
   </si>
   <si>
     <t>17 Jun 17.07</t>
@@ -1217,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1305,9 +1302,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1723,127 +1717,127 @@
   <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T70" sqref="T70"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="3"/>
+    <col min="1" max="1" width="9.1015625" style="3"/>
     <col min="2" max="2" width="20" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.08984375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.31640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="4.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.31640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.08984375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.08984375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="3.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1015625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="26.47265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.1015625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.3125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="4.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.3125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1015625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.1015625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="3.5234375" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.453125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="15.453125" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.08984375" style="2"/>
+    <col min="14" max="14" width="5.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="12.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.47265625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="15.47265625" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.1015625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="49" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="48" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="51" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="46" t="s">
         <v>327</v>
       </c>
-      <c r="F1" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="47" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="49"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="36" t="s">
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="48"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="46" t="s">
+      <c r="O2" s="45" t="s">
+        <v>319</v>
+      </c>
+      <c r="P2" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="P2" s="46" t="s">
-        <v>321</v>
-      </c>
-      <c r="Q2" s="36" t="s">
+      <c r="Q2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="50"/>
-      <c r="T2" s="48"/>
-    </row>
-    <row r="3" spans="1:20" s="20" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="S2" s="49"/>
+      <c r="T2" s="47"/>
+    </row>
+    <row r="3" spans="1:20" s="20" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>27</v>
@@ -1873,24 +1867,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="20" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:20" s="20" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C4" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D4" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>260</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>261</v>
       </c>
       <c r="G4" s="13">
         <v>6</v>
@@ -1926,16 +1920,16 @@
         <v>27</v>
       </c>
       <c r="R4" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="S4" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="S4" s="13" t="s">
-        <v>263</v>
-      </c>
       <c r="T4" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="20" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:20" s="20" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -1986,7 +1980,7 @@
         <v>27</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S5" s="13" t="s">
         <v>106</v>
@@ -1995,24 +1989,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="20" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:20" s="20" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>269</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>270</v>
       </c>
       <c r="G6" s="13">
         <v>4</v>
@@ -2049,30 +2043,30 @@
       </c>
       <c r="R6" s="19"/>
       <c r="S6" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="T6" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" s="34">
+        <v>196</v>
+      </c>
+      <c r="C7" s="33">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>198</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>199</v>
       </c>
       <c r="G7" s="13">
         <v>3</v>
@@ -2093,13 +2087,13 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="19"/>
       <c r="S7" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T7" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -2155,12 +2149,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:20" s="20" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="13">
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" s="17">
         <v>4.2361111111111106E-2</v>
@@ -2172,7 +2166,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G9" s="13">
         <v>2</v>
@@ -2200,93 +2194,93 @@
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="S9" s="32" t="s">
-        <v>278</v>
+        <v>263</v>
+      </c>
+      <c r="S9" s="31" t="s">
+        <v>277</v>
       </c>
       <c r="T9" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="20" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:20" s="20" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="13">
         <v>8</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10" s="34">
+        <v>184</v>
+      </c>
+      <c r="C10" s="33">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D10" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="G10" s="13">
-        <v>2</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="R10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="13" t="s">
-        <v>160</v>
-      </c>
       <c r="T10" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="20" customFormat="1" ht="170.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:20" s="20" customFormat="1" ht="170.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6">
         <v>9</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G11" s="6">
         <v>2</v>
@@ -2310,33 +2304,33 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="T11" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="13">
         <v>10</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C12" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D12" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="F12" s="18" t="s">
         <v>228</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>229</v>
       </c>
       <c r="G12" s="13">
         <v>2</v>
@@ -2357,20 +2351,20 @@
       <c r="Q12" s="13"/>
       <c r="R12" s="19"/>
       <c r="S12" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T12" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="13">
         <v>11</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>282</v>
-      </c>
-      <c r="C13" s="34">
+        <v>281</v>
+      </c>
+      <c r="C13" s="33">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -2423,24 +2417,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:20" s="20" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="13">
         <v>12</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="34">
+        <v>131</v>
+      </c>
+      <c r="C14" s="33">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D14" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="F14" s="18" t="s">
         <v>128</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>129</v>
       </c>
       <c r="G14" s="13">
         <v>3</v>
@@ -2452,47 +2446,47 @@
         <v>27</v>
       </c>
       <c r="J14" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="K14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="R14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="S14" s="13" t="s">
-        <v>131</v>
-      </c>
       <c r="T14" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="20" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:20" s="20" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="13">
         <v>13</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="C15" s="34">
+        <v>180</v>
+      </c>
+      <c r="C15" s="33">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D15" s="18" t="s">
@@ -2543,12 +2537,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="20" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:20" s="20" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="13">
         <v>14</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="17">
         <v>4.2361111111111106E-2</v>
@@ -2560,7 +2554,7 @@
         <v>6</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G16" s="13">
         <v>2</v>
@@ -2585,30 +2579,30 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="19"/>
       <c r="S16" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T16" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="20" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:20" s="20" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="13">
         <v>15</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="C17" s="34">
+        <v>234</v>
+      </c>
+      <c r="C17" s="33">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G17" s="13">
         <v>3</v>
@@ -2631,19 +2625,19 @@
         <v>27</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T17" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="20" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:20" s="20" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="13">
         <v>16</v>
       </c>
@@ -2701,7 +2695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="20" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:20" s="20" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="13">
         <v>17</v>
       </c>
@@ -2759,7 +2753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="13">
         <v>18</v>
       </c>
@@ -2817,12 +2811,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="24">
         <v>19</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C21" s="26">
         <v>4.2361111111111106E-2</v>
@@ -2834,7 +2828,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G21" s="24">
         <v>2</v>
@@ -2862,7 +2856,7 @@
         <v>27</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="S21" s="28">
         <v>43649</v>
@@ -2871,12 +2865,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:20" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="13">
         <v>20</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>27</v>
@@ -2924,31 +2918,31 @@
         <v>27</v>
       </c>
       <c r="R22" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="S22" s="33" t="s">
-        <v>275</v>
+        <v>322</v>
+      </c>
+      <c r="S22" s="32" t="s">
+        <v>274</v>
       </c>
       <c r="T22" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="20" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:20" s="20" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="13">
         <v>21</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="F23" s="18" t="s">
         <v>213</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>214</v>
       </c>
       <c r="G23" s="13">
         <v>2</v>
@@ -2969,13 +2963,13 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="19"/>
       <c r="S23" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T23" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="29" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:20" s="29" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="13">
         <v>22</v>
       </c>
@@ -2986,7 +2980,7 @@
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>60</v>
@@ -3026,7 +3020,7 @@
         <v>27</v>
       </c>
       <c r="R24" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="S24" s="13" t="s">
         <v>62</v>
@@ -3035,12 +3029,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="13">
         <v>23</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="17" t="s">
@@ -3071,18 +3065,18 @@
       <c r="Q25" s="13"/>
       <c r="R25" s="19"/>
       <c r="S25" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="T25" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:20" s="20" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="13">
         <v>24</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="17" t="s">
@@ -3115,28 +3109,28 @@
       <c r="Q26" s="13"/>
       <c r="R26" s="19"/>
       <c r="S26" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T26" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="13">
         <v>25</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G27" s="13">
         <v>2</v>
@@ -3157,28 +3151,28 @@
       <c r="Q27" s="13"/>
       <c r="R27" s="19"/>
       <c r="S27" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T27" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="13">
         <v>26</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="C28" s="34"/>
+        <v>170</v>
+      </c>
+      <c r="C28" s="33"/>
       <c r="D28" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G28" s="13">
         <v>1</v>
@@ -3201,36 +3195,36 @@
         <v>27</v>
       </c>
       <c r="Q28" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R28" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S28" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T28" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:20" s="20" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="13">
         <v>27</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D29" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="F29" s="18" t="s">
         <v>140</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>141</v>
       </c>
       <c r="G29" s="13">
         <v>2</v>
@@ -3267,18 +3261,18 @@
       </c>
       <c r="R29" s="19"/>
       <c r="S29" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T29" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="20" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:20" s="20" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="13">
         <v>28</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="17" t="s">
@@ -3331,7 +3325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="13">
         <v>29</v>
       </c>
@@ -3389,24 +3383,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="13">
         <v>30</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>220</v>
-      </c>
       <c r="D32" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>72</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G32" s="13">
         <v>2</v>
@@ -3427,30 +3421,30 @@
       <c r="Q32" s="13"/>
       <c r="R32" s="19"/>
       <c r="S32" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="T32" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="13">
         <v>31</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C33" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>111</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G33" s="13">
         <v>3</v>
@@ -3487,30 +3481,30 @@
       </c>
       <c r="R33" s="19"/>
       <c r="S33" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T33" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="13">
         <v>32</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D34" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>146</v>
-      </c>
       <c r="F34" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G34" s="13">
         <v>2</v>
@@ -3522,7 +3516,7 @@
         <v>4</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K34" s="13">
         <v>1</v>
@@ -3546,33 +3540,33 @@
         <v>27</v>
       </c>
       <c r="R34" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S34" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T34" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="13">
         <v>33</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D35" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="F35" s="18" t="s">
         <v>168</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>169</v>
       </c>
       <c r="G35" s="13">
         <v>2</v>
@@ -3598,16 +3592,16 @@
         <v>27</v>
       </c>
       <c r="R35" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="S35" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T35" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="13">
         <v>34</v>
       </c>
@@ -3667,7 +3661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="13">
         <v>35</v>
       </c>
@@ -3678,7 +3672,7 @@
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>46</v>
@@ -3725,24 +3719,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="13">
         <v>36</v>
       </c>
       <c r="B38" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="D38" s="17" t="s">
         <v>231</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>232</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G38" s="13">
         <v>4</v>
@@ -3766,21 +3760,21 @@
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T38" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="13">
         <v>37</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C39" s="17">
         <v>4.2361111111111106E-2</v>
@@ -3792,7 +3786,7 @@
         <v>16</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G39" s="13">
         <v>2</v>
@@ -3813,27 +3807,27 @@
       <c r="Q39" s="13"/>
       <c r="R39" s="19"/>
       <c r="S39" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T39" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="13">
         <v>38</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="33" t="s">
         <v>63</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="30" t="s">
-        <v>125</v>
+      <c r="E40" s="27" t="s">
+        <v>314</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>24</v>
@@ -3867,17 +3861,17 @@
       <c r="Q40" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R40" s="31" t="s">
-        <v>299</v>
+      <c r="R40" s="30" t="s">
+        <v>298</v>
       </c>
       <c r="S40" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T40" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="13">
         <v>39</v>
       </c>
@@ -3933,7 +3927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="13">
         <v>40</v>
       </c>
@@ -3987,7 +3981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="13">
         <v>41</v>
       </c>
@@ -4036,7 +4030,7 @@
         <v>2</v>
       </c>
       <c r="R43" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S43" s="13" t="s">
         <v>76</v>
@@ -4045,21 +4039,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="13">
         <v>42</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="C44" s="34">
+        <v>284</v>
+      </c>
+      <c r="C44" s="33">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>83</v>
@@ -4105,12 +4099,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="13">
         <v>43</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="17" t="s">
@@ -4132,7 +4126,7 @@
         <v>1</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K45" s="13">
         <v>1</v>
@@ -4165,7 +4159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="13">
         <v>44</v>
       </c>
@@ -4223,22 +4217,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="20" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:20" s="20" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="13">
         <v>45</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>21</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G47" s="13">
         <v>4</v>
@@ -4272,16 +4266,16 @@
         <v>27</v>
       </c>
       <c r="R47" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S47" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T47" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="13">
         <v>46</v>
       </c>
@@ -4337,19 +4331,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="13">
         <v>47</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F49" s="18"/>
       <c r="G49" s="13">
@@ -4387,13 +4381,13 @@
       </c>
       <c r="R49" s="19"/>
       <c r="S49" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T49" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="13">
         <v>48</v>
       </c>
@@ -4449,7 +4443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="20" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:20" s="20" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="13">
         <v>49</v>
       </c>
@@ -4505,22 +4499,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="13">
         <v>50</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>20</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G52" s="13">
         <v>1</v>
@@ -4541,18 +4535,18 @@
       <c r="Q52" s="13"/>
       <c r="R52" s="19"/>
       <c r="S52" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T52" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="13">
         <v>51</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C53" s="17">
         <v>4.2361111111111106E-2</v>
@@ -4564,7 +4558,7 @@
         <v>16</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G53" s="13">
         <v>2</v>
@@ -4585,18 +4579,18 @@
       <c r="Q53" s="13"/>
       <c r="R53" s="19"/>
       <c r="S53" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T53" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="13">
         <v>52</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18" t="s">
@@ -4643,18 +4637,18 @@
       </c>
       <c r="R54" s="19"/>
       <c r="S54" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="T54" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:20" s="20" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="13">
         <v>53</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C55" s="17">
         <v>4.2361111111111106E-2</v>
@@ -4709,16 +4703,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:20" s="20" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:20" s="20" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="13">
         <v>54</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E56" s="18" t="s">
         <v>16</v>
@@ -4757,24 +4751,24 @@
         <v>27</v>
       </c>
       <c r="Q56" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="R56" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="R56" s="19" t="s">
-        <v>290</v>
-      </c>
       <c r="S56" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T56" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="13">
         <v>55</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="17" t="s">
@@ -4784,7 +4778,7 @@
         <v>22</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G57" s="13">
         <v>2</v>
@@ -4805,30 +4799,30 @@
       <c r="Q57" s="13"/>
       <c r="R57" s="19"/>
       <c r="S57" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T57" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="13">
         <v>56</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C58" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="F58" s="35" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="F58" s="34" t="s">
+        <v>207</v>
       </c>
       <c r="G58" s="13">
         <v>2</v>
@@ -4850,16 +4844,16 @@
       <c r="P58" s="13"/>
       <c r="Q58" s="13"/>
       <c r="R58" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S58" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="T58" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="13">
         <v>57</v>
       </c>
@@ -4910,7 +4904,7 @@
         <v>27</v>
       </c>
       <c r="R59" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S59" s="13" t="s">
         <v>123</v>
@@ -4919,18 +4913,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="13">
         <v>58</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>16</v>
@@ -4968,21 +4962,21 @@
         <v>27</v>
       </c>
       <c r="R60" s="19" t="s">
-        <v>325</v>
-      </c>
-      <c r="S60" s="33" t="s">
-        <v>280</v>
+        <v>324</v>
+      </c>
+      <c r="S60" s="32" t="s">
+        <v>279</v>
       </c>
       <c r="T60" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="13">
         <v>59</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="18" t="s">
@@ -4992,7 +4986,7 @@
         <v>22</v>
       </c>
       <c r="F61" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G61" s="13">
         <v>2</v>
@@ -5012,19 +5006,19 @@
       <c r="P61" s="13"/>
       <c r="Q61" s="13"/>
       <c r="R61" s="19"/>
-      <c r="S61" s="33" t="s">
-        <v>306</v>
+      <c r="S61" s="32" t="s">
+        <v>305</v>
       </c>
       <c r="T61" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:20" s="20" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:20" s="20" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="6">
         <v>60</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -5032,7 +5026,7 @@
         <v>16</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G62" s="6">
         <v>2</v>
@@ -5059,12 +5053,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:20" s="20" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:20" s="20" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="13">
         <v>61</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C63" s="17">
         <v>4.2361111111111106E-2</v>
@@ -5073,10 +5067,10 @@
         <v>96</v>
       </c>
       <c r="E63" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="F63" s="18" t="s">
         <v>155</v>
-      </c>
-      <c r="F63" s="18" t="s">
-        <v>156</v>
       </c>
       <c r="G63" s="13">
         <v>2</v>
@@ -5086,7 +5080,7 @@
       </c>
       <c r="I63" s="13"/>
       <c r="J63" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K63" s="13" t="s">
         <v>27</v>
@@ -5110,33 +5104,33 @@
         <v>27</v>
       </c>
       <c r="R63" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T63" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="13">
         <v>62</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C64" s="17">
         <v>4.2361111111111106E-2</v>
       </c>
       <c r="D64" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="F64" s="18" t="s">
         <v>135</v>
-      </c>
-      <c r="F64" s="18" t="s">
-        <v>136</v>
       </c>
       <c r="G64" s="13">
         <v>4</v>
@@ -5148,45 +5142,45 @@
         <v>1</v>
       </c>
       <c r="J64" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K64" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L64" s="13">
+        <v>1</v>
+      </c>
+      <c r="M64" s="13">
+        <v>1</v>
+      </c>
+      <c r="N64" s="13">
+        <v>2</v>
+      </c>
+      <c r="O64" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P64" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q64" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="R64" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="S64" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="K64" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L64" s="13">
-        <v>1</v>
-      </c>
-      <c r="M64" s="13">
-        <v>1</v>
-      </c>
-      <c r="N64" s="13">
-        <v>2</v>
-      </c>
-      <c r="O64" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P64" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q64" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="R64" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="S64" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="T64" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="13">
         <v>63</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C65" s="17">
         <v>4.2361111111111106E-2</v>
@@ -5195,10 +5189,10 @@
         <v>96</v>
       </c>
       <c r="E65" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F65" s="18" t="s">
         <v>187</v>
-      </c>
-      <c r="F65" s="18" t="s">
-        <v>188</v>
       </c>
       <c r="G65" s="13">
         <v>3</v>
@@ -5221,13 +5215,13 @@
       <c r="Q65" s="13"/>
       <c r="R65" s="19"/>
       <c r="S65" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T65" s="20">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="13">
         <v>64</v>
       </c>
@@ -5287,16 +5281,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:20" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="13">
         <v>65</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E67" s="18" t="s">
         <v>16</v>
@@ -5336,21 +5330,21 @@
         <v>27</v>
       </c>
       <c r="R67" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="S67" s="13" t="s">
         <v>245</v>
-      </c>
-      <c r="S67" s="13" t="s">
-        <v>246</v>
       </c>
       <c r="T67" s="20">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="13">
         <v>66</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C68" s="17">
         <v>4.2361111111111106E-2</v>
@@ -5359,10 +5353,10 @@
         <v>96</v>
       </c>
       <c r="E68" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="F68" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="F68" s="18" t="s">
-        <v>150</v>
       </c>
       <c r="G68" s="13">
         <v>2</v>
@@ -5387,24 +5381,24 @@
       </c>
       <c r="P68" s="13"/>
       <c r="Q68" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R68" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S68" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T68" s="20">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="13">
         <v>67</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>27</v>
@@ -5450,7 +5444,7 @@
         <v>27</v>
       </c>
       <c r="R69" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="S69" s="13" t="s">
         <v>27</v>
@@ -5459,7 +5453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:20" ht="66" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="13">
         <v>68</v>
       </c>
@@ -5519,7 +5513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="6"/>
       <c r="B71" s="11" t="s">
         <v>11</v>
@@ -5606,566 +5600,566 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="41" customWidth="1"/>
-    <col min="2" max="2" width="66.08984375" style="45" customWidth="1"/>
-    <col min="3" max="16384" width="9.08984375" style="37"/>
+    <col min="1" max="1" width="10.1015625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="66.1015625" style="44" customWidth="1"/>
+    <col min="3" max="16384" width="9.1015625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A1" s="54" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="55" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A2" s="54"/>
-      <c r="B2" s="55"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A3" s="38">
-        <v>1</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A4" s="39">
-        <v>2</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A5" s="39">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="37">
+        <v>1</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="38">
+        <v>2</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="38">
         <v>3</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A6" s="39">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="38">
         <v>4</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A7" s="39">
+      <c r="B6" s="42" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="38">
         <v>5</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A8" s="39">
+      <c r="B7" s="42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="38">
         <v>6</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A9" s="39">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="38">
         <v>7</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A10" s="39">
+      <c r="B9" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="38">
         <v>8</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="37">
+        <v>9</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="38">
+        <v>10</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" s="38">
+        <v>11</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" s="38">
+        <v>12</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" s="38">
+        <v>13</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" s="38">
+        <v>14</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="38">
+        <v>15</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="38">
+        <v>16</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="38">
+        <v>17</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="38">
+        <v>18</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="39">
+        <v>19</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="38">
+        <v>20</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="38">
+        <v>21</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="38">
+        <v>22</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="38">
+        <v>23</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="38">
+        <v>24</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="38">
+        <v>25</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="38">
+        <v>26</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="38">
+        <v>27</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="38">
+        <v>28</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="38">
+        <v>29</v>
+      </c>
+      <c r="B31" s="42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="38">
+        <v>30</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="38">
+        <v>31</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="38">
+        <v>32</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="38">
+        <v>33</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36" s="38">
+        <v>34</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37" s="38">
+        <v>35</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38" s="38">
+        <v>36</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39" s="38">
+        <v>37</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40" s="38">
+        <v>38</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41" s="38">
+        <v>39</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42" s="38">
+        <v>40</v>
+      </c>
+      <c r="B42" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43" s="38">
+        <v>41</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44" s="38">
+        <v>42</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45" s="38">
+        <v>43</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46" s="38">
+        <v>44</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47" s="38">
+        <v>45</v>
+      </c>
+      <c r="B47" s="42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48" s="38">
+        <v>46</v>
+      </c>
+      <c r="B48" s="42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49" s="38">
+        <v>47</v>
+      </c>
+      <c r="B49" s="42" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A50" s="38">
+        <v>48</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A51" s="38">
+        <v>49</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A52" s="38">
+        <v>50</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A53" s="38">
+        <v>51</v>
+      </c>
+      <c r="B53" s="42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A54" s="38">
+        <v>52</v>
+      </c>
+      <c r="B54" s="42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A55" s="38">
+        <v>53</v>
+      </c>
+      <c r="B55" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A56" s="38">
+        <v>54</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A57" s="38">
+        <v>55</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A58" s="38">
+        <v>56</v>
+      </c>
+      <c r="B58" s="42" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A59" s="38">
+        <v>57</v>
+      </c>
+      <c r="B59" s="42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A60" s="38">
+        <v>58</v>
+      </c>
+      <c r="B60" s="42" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A61" s="38">
+        <v>59</v>
+      </c>
+      <c r="B61" s="42" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A62" s="37">
+        <v>60</v>
+      </c>
+      <c r="B62" s="41" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A63" s="38">
+        <v>61</v>
+      </c>
+      <c r="B63" s="42" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A11" s="38">
-        <v>9</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A12" s="39">
-        <v>10</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A13" s="39">
-        <v>11</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A14" s="39">
-        <v>12</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A15" s="39">
-        <v>13</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A16" s="39">
-        <v>14</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A17" s="39">
-        <v>15</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A18" s="39">
-        <v>16</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A19" s="39">
-        <v>17</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A20" s="39">
-        <v>18</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A21" s="40">
-        <v>19</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A22" s="39">
-        <v>20</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A23" s="39">
-        <v>21</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A24" s="39">
-        <v>22</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A25" s="39">
-        <v>23</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A26" s="39">
-        <v>24</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A27" s="39">
-        <v>25</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A28" s="39">
-        <v>26</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A29" s="39">
-        <v>27</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A30" s="39">
-        <v>28</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A31" s="39">
-        <v>29</v>
-      </c>
-      <c r="B31" s="43" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A32" s="39">
-        <v>30</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A33" s="39">
-        <v>31</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A34" s="39">
-        <v>32</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A35" s="39">
-        <v>33</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A36" s="39">
-        <v>34</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A37" s="39">
-        <v>35</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A38" s="39">
-        <v>36</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A39" s="39">
-        <v>37</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A40" s="39">
-        <v>38</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A41" s="39">
-        <v>39</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A42" s="39">
-        <v>40</v>
-      </c>
-      <c r="B42" s="43" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A64" s="38">
+        <v>62</v>
+      </c>
+      <c r="B64" s="42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A65" s="38">
+        <v>63</v>
+      </c>
+      <c r="B65" s="42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A66" s="38">
         <v>64</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A43" s="39">
-        <v>41</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A44" s="39">
-        <v>42</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A45" s="39">
-        <v>43</v>
-      </c>
-      <c r="B45" s="43" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A46" s="39">
-        <v>44</v>
-      </c>
-      <c r="B46" s="43" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A47" s="39">
-        <v>45</v>
-      </c>
-      <c r="B47" s="43" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A48" s="39">
-        <v>46</v>
-      </c>
-      <c r="B48" s="43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A49" s="39">
-        <v>47</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A50" s="39">
-        <v>48</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A51" s="39">
-        <v>49</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A52" s="39">
-        <v>50</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A53" s="39">
-        <v>51</v>
-      </c>
-      <c r="B53" s="43" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A54" s="39">
-        <v>52</v>
-      </c>
-      <c r="B54" s="43" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A55" s="39">
-        <v>53</v>
-      </c>
-      <c r="B55" s="43" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A56" s="39">
-        <v>54</v>
-      </c>
-      <c r="B56" s="43" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A57" s="39">
-        <v>55</v>
-      </c>
-      <c r="B57" s="43" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A58" s="39">
-        <v>56</v>
-      </c>
-      <c r="B58" s="43" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A59" s="39">
-        <v>57</v>
-      </c>
-      <c r="B59" s="43" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A60" s="39">
-        <v>58</v>
-      </c>
-      <c r="B60" s="43" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A61" s="39">
-        <v>59</v>
-      </c>
-      <c r="B61" s="43" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A62" s="38">
-        <v>60</v>
-      </c>
-      <c r="B62" s="42" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A63" s="39">
-        <v>61</v>
-      </c>
-      <c r="B63" s="43" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A64" s="39">
-        <v>62</v>
-      </c>
-      <c r="B64" s="43" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A65" s="39">
-        <v>63</v>
-      </c>
-      <c r="B65" s="43" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A66" s="39">
-        <v>64</v>
-      </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="42" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A67" s="39">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A67" s="38">
         <v>65</v>
       </c>
-      <c r="B67" s="43" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A68" s="39">
+      <c r="B67" s="42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68" s="38">
         <v>66</v>
       </c>
-      <c r="B68" s="43" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A69" s="39">
+      <c r="B68" s="42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69" s="38">
         <v>67</v>
       </c>
-      <c r="B69" s="43" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A70" s="39">
+      <c r="B69" s="42" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70" s="38">
         <v>68</v>
       </c>
-      <c r="B70" s="43" t="s">
+      <c r="B70" s="42" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>